<commit_message>
first submit when go back
</commit_message>
<xml_diff>
--- a/training/imdb/metadata.xlsx
+++ b/training/imdb/metadata.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\something\talq\zebura_lit\training\imdb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E42A467-61EA-418E-96F3-B1C7101266F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
     <sheet name="tables" sheetId="2" r:id="rId2"/>
     <sheet name="fields" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="87">
-  <si>
-    <t>database_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>domain</t>
   </si>
@@ -307,16 +310,31 @@
   <si>
     <t>0.0, 68.0, 72.0, 66.0, 64.0, 57.0, 65.0, 51.0, 76.0, 81.0</t>
   </si>
+  <si>
+    <t>database_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tags</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>examples</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hypernym</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -324,8 +342,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -337,7 +362,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -360,28 +385,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -419,7 +469,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -453,6 +503,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -487,9 +538,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -662,458 +714,486 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>255</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>255</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>255</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>255</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7">
         <v>255</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>